<commit_message>
Changes made:   - added calculation for columns containing normalized FTE;   - the sequence of rounding of actual FTE has been changed.
</commit_message>
<xml_diff>
--- a/Settings.xlsx
+++ b/Settings.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7605142E-7622-42FE-BF4C-C4DF2010EA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1553534F-A77C-49D8-9F76-6BB1F68DC93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -384,7 +384,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>